<commit_message>
update readme - output analysis
</commit_message>
<xml_diff>
--- a/ISI_TUPF_3.xlsx
+++ b/ISI_TUPF_3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I166"/>
+  <dimension ref="A1:J166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,6 +474,11 @@
           <t>Mg/Ca-SWT</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 8</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -505,6 +510,7 @@
       <c r="I2" t="n">
         <v>-1.97</v>
       </c>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -536,6 +542,7 @@
       <c r="I3" t="n">
         <v>-6.25</v>
       </c>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -567,6 +574,7 @@
       <c r="I4" t="n">
         <v>-6.66</v>
       </c>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -598,6 +606,7 @@
       <c r="I5" t="n">
         <v>-5.95</v>
       </c>
+      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -629,6 +638,7 @@
       <c r="I6" t="n">
         <v>-6.29</v>
       </c>
+      <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -660,6 +670,7 @@
       <c r="I7" t="n">
         <v>-6.75</v>
       </c>
+      <c r="J7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -691,6 +702,7 @@
       <c r="I8" t="n">
         <v>-7.59</v>
       </c>
+      <c r="J8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -722,6 +734,7 @@
       <c r="I9" t="n">
         <v>-7.5</v>
       </c>
+      <c r="J9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -753,6 +766,7 @@
       <c r="I10" t="n">
         <v>-7.5</v>
       </c>
+      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -784,6 +798,7 @@
       <c r="I11" t="n">
         <v>-8.41</v>
       </c>
+      <c r="J11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -815,6 +830,7 @@
       <c r="I12" t="n">
         <v>-4.84</v>
       </c>
+      <c r="J12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -846,6 +862,7 @@
       <c r="I13" t="n">
         <v>-36.56</v>
       </c>
+      <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -877,6 +894,7 @@
       <c r="I14" t="n">
         <v>-31.16</v>
       </c>
+      <c r="J14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -908,6 +926,7 @@
       <c r="I15" t="n">
         <v>-35.14</v>
       </c>
+      <c r="J15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -939,6 +958,7 @@
       <c r="I16" t="n">
         <v>-36.71</v>
       </c>
+      <c r="J16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -970,6 +990,7 @@
       <c r="I17" t="n">
         <v>-36.37</v>
       </c>
+      <c r="J17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1001,6 +1022,7 @@
       <c r="I18" t="n">
         <v>-36.18</v>
       </c>
+      <c r="J18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1032,6 +1054,7 @@
       <c r="I19" t="n">
         <v>-2.76</v>
       </c>
+      <c r="J19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1063,6 +1086,7 @@
       <c r="I20" t="n">
         <v>-5.46</v>
       </c>
+      <c r="J20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1094,6 +1118,7 @@
       <c r="I21" t="n">
         <v>-0.93</v>
       </c>
+      <c r="J21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1125,6 +1150,7 @@
       <c r="I22" t="n">
         <v>-3.77</v>
       </c>
+      <c r="J22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1156,6 +1182,7 @@
       <c r="I23" t="n">
         <v>-0.55</v>
       </c>
+      <c r="J23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1187,6 +1214,7 @@
       <c r="I24" t="n">
         <v>-8.359999999999999</v>
       </c>
+      <c r="J24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1218,6 +1246,7 @@
       <c r="I25" t="n">
         <v>-4.46</v>
       </c>
+      <c r="J25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1249,6 +1278,7 @@
       <c r="I26" t="n">
         <v>-5.16</v>
       </c>
+      <c r="J26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1280,6 +1310,7 @@
       <c r="I27" t="n">
         <v>-8.539999999999999</v>
       </c>
+      <c r="J27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1311,6 +1342,7 @@
       <c r="I28" t="n">
         <v>-4.81</v>
       </c>
+      <c r="J28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1342,6 +1374,7 @@
       <c r="I29" t="n">
         <v>-6.96</v>
       </c>
+      <c r="J29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1373,6 +1406,7 @@
       <c r="I30" t="n">
         <v>-4.7</v>
       </c>
+      <c r="J30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1404,6 +1438,7 @@
       <c r="I31" t="n">
         <v>0.01</v>
       </c>
+      <c r="J31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1435,6 +1470,7 @@
       <c r="I32" t="n">
         <v>-7.18</v>
       </c>
+      <c r="J32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1466,6 +1502,7 @@
       <c r="I33" t="n">
         <v>30.69</v>
       </c>
+      <c r="J33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1497,6 +1534,7 @@
       <c r="I34" t="n">
         <v>-8.07</v>
       </c>
+      <c r="J34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1528,6 +1566,7 @@
       <c r="I35" t="n">
         <v>-4.33</v>
       </c>
+      <c r="J35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1559,6 +1598,7 @@
       <c r="I36" t="n">
         <v>-6.57</v>
       </c>
+      <c r="J36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1590,6 +1630,7 @@
       <c r="I37" t="n">
         <v>-4.19</v>
       </c>
+      <c r="J37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1621,6 +1662,7 @@
       <c r="I38" t="n">
         <v>-1.5</v>
       </c>
+      <c r="J38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1652,6 +1694,7 @@
       <c r="I39" t="n">
         <v>-4.65</v>
       </c>
+      <c r="J39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -1683,6 +1726,7 @@
       <c r="I40" t="n">
         <v>-4.21</v>
       </c>
+      <c r="J40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -1714,6 +1758,7 @@
       <c r="I41" t="n">
         <v>-5.23</v>
       </c>
+      <c r="J41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -1745,6 +1790,7 @@
       <c r="I42" t="n">
         <v>-4.6</v>
       </c>
+      <c r="J42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1776,6 +1822,7 @@
       <c r="I43" t="n">
         <v>-3.53</v>
       </c>
+      <c r="J43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1807,6 +1854,7 @@
       <c r="I44" t="n">
         <v>1.39</v>
       </c>
+      <c r="J44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -1838,6 +1886,7 @@
       <c r="I45" t="n">
         <v>3.02</v>
       </c>
+      <c r="J45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -1869,6 +1918,7 @@
       <c r="I46" t="n">
         <v>-1.14</v>
       </c>
+      <c r="J46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -1900,6 +1950,7 @@
       <c r="I47" t="n">
         <v>-2.78</v>
       </c>
+      <c r="J47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -1931,6 +1982,7 @@
       <c r="I48" t="n">
         <v>8.9</v>
       </c>
+      <c r="J48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -1962,6 +2014,7 @@
       <c r="I49" t="n">
         <v>-0.1</v>
       </c>
+      <c r="J49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -1993,6 +2046,7 @@
       <c r="I50" t="n">
         <v>-0.22</v>
       </c>
+      <c r="J50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -2024,6 +2078,7 @@
       <c r="I51" t="n">
         <v>-3.97</v>
       </c>
+      <c r="J51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -2055,6 +2110,7 @@
       <c r="I52" t="n">
         <v>-3.85</v>
       </c>
+      <c r="J52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -2086,6 +2142,7 @@
       <c r="I53" t="n">
         <v>6.58</v>
       </c>
+      <c r="J53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -2117,6 +2174,7 @@
       <c r="I54" t="n">
         <v>13.89</v>
       </c>
+      <c r="J54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -2148,6 +2206,7 @@
       <c r="I55" t="n">
         <v>7.29</v>
       </c>
+      <c r="J55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -2179,6 +2238,7 @@
       <c r="I56" t="n">
         <v>1.87</v>
       </c>
+      <c r="J56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -2210,6 +2270,7 @@
       <c r="I57" t="n">
         <v>-3.86</v>
       </c>
+      <c r="J57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -2241,6 +2302,7 @@
       <c r="I58" t="n">
         <v>6.28</v>
       </c>
+      <c r="J58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -2272,6 +2334,7 @@
       <c r="I59" t="n">
         <v>-4.15</v>
       </c>
+      <c r="J59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -2303,6 +2366,7 @@
       <c r="I60" t="n">
         <v>-3.42</v>
       </c>
+      <c r="J60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -2334,6 +2398,7 @@
       <c r="I61" t="n">
         <v>-5.95</v>
       </c>
+      <c r="J61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -2365,6 +2430,7 @@
       <c r="I62" t="n">
         <v>1.33</v>
       </c>
+      <c r="J62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -2396,6 +2462,7 @@
       <c r="I63" t="n">
         <v>-5.57</v>
       </c>
+      <c r="J63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -2427,6 +2494,7 @@
       <c r="I64" t="n">
         <v>5.1</v>
       </c>
+      <c r="J64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -2458,6 +2526,7 @@
       <c r="I65" t="n">
         <v>-2.95</v>
       </c>
+      <c r="J65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -2489,6 +2558,7 @@
       <c r="I66" t="n">
         <v>4.75</v>
       </c>
+      <c r="J66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -2520,6 +2590,7 @@
       <c r="I67" t="n">
         <v>-8.880000000000001</v>
       </c>
+      <c r="J67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -2551,6 +2622,7 @@
       <c r="I68" t="n">
         <v>-7.45</v>
       </c>
+      <c r="J68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -2582,6 +2654,7 @@
       <c r="I69" t="n">
         <v>-1.78</v>
       </c>
+      <c r="J69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -2613,6 +2686,7 @@
       <c r="I70" t="n">
         <v>14.25</v>
       </c>
+      <c r="J70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -2644,6 +2718,7 @@
       <c r="I71" t="n">
         <v>-13.13</v>
       </c>
+      <c r="J71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -2675,6 +2750,7 @@
       <c r="I72" t="n">
         <v>13.75</v>
       </c>
+      <c r="J72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -2706,6 +2782,7 @@
       <c r="I73" t="n">
         <v>-15.97</v>
       </c>
+      <c r="J73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -2737,6 +2814,7 @@
       <c r="I74" t="n">
         <v>-15.89</v>
       </c>
+      <c r="J74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -2768,6 +2846,7 @@
       <c r="I75" t="n">
         <v>-14.34</v>
       </c>
+      <c r="J75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -2799,6 +2878,7 @@
       <c r="I76" t="n">
         <v>4.68</v>
       </c>
+      <c r="J76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -2830,6 +2910,7 @@
       <c r="I77" t="n">
         <v>5.12</v>
       </c>
+      <c r="J77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -2861,6 +2942,7 @@
       <c r="I78" t="n">
         <v>7.58</v>
       </c>
+      <c r="J78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -2892,6 +2974,7 @@
       <c r="I79" t="n">
         <v>6.14</v>
       </c>
+      <c r="J79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -2923,6 +3006,7 @@
       <c r="I80" t="n">
         <v>11.23</v>
       </c>
+      <c r="J80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -2954,6 +3038,7 @@
       <c r="I81" t="n">
         <v>1.51</v>
       </c>
+      <c r="J81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -2985,6 +3070,7 @@
       <c r="I82" t="n">
         <v>36.32</v>
       </c>
+      <c r="J82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -3016,6 +3102,7 @@
       <c r="I83" t="n">
         <v>70.7</v>
       </c>
+      <c r="J83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -3047,6 +3134,7 @@
       <c r="I84" t="n">
         <v>-5.04</v>
       </c>
+      <c r="J84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -3078,6 +3166,7 @@
       <c r="I85" t="n">
         <v>-8.43</v>
       </c>
+      <c r="J85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -3109,6 +3198,7 @@
       <c r="I86" t="n">
         <v>-7.8</v>
       </c>
+      <c r="J86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -3140,6 +3230,7 @@
       <c r="I87" t="n">
         <v>-8.02</v>
       </c>
+      <c r="J87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -3171,6 +3262,7 @@
       <c r="I88" t="n">
         <v>-6.71</v>
       </c>
+      <c r="J88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -3202,6 +3294,7 @@
       <c r="I89" t="n">
         <v>-7.22</v>
       </c>
+      <c r="J89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -3233,6 +3326,7 @@
       <c r="I90" t="n">
         <v>17.31</v>
       </c>
+      <c r="J90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -3264,6 +3358,7 @@
       <c r="I91" t="n">
         <v>-0.5600000000000001</v>
       </c>
+      <c r="J91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -3295,6 +3390,7 @@
       <c r="I92" t="n">
         <v>-1.4</v>
       </c>
+      <c r="J92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -3326,6 +3422,7 @@
       <c r="I93" t="n">
         <v>-5.16</v>
       </c>
+      <c r="J93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -3357,6 +3454,7 @@
       <c r="I94" t="n">
         <v>-5.81</v>
       </c>
+      <c r="J94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -3388,6 +3486,7 @@
       <c r="I95" t="n">
         <v>-5.12</v>
       </c>
+      <c r="J95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -3419,6 +3518,7 @@
       <c r="I96" t="n">
         <v>-6.61</v>
       </c>
+      <c r="J96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -3450,6 +3550,7 @@
       <c r="I97" t="n">
         <v>-7.93</v>
       </c>
+      <c r="J97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -3481,6 +3582,7 @@
       <c r="I98" t="n">
         <v>-6.88</v>
       </c>
+      <c r="J98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -3512,6 +3614,7 @@
       <c r="I99" t="n">
         <v>-1.99</v>
       </c>
+      <c r="J99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -3543,6 +3646,7 @@
       <c r="I100" t="n">
         <v>1.22</v>
       </c>
+      <c r="J100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -3574,6 +3678,7 @@
       <c r="I101" t="n">
         <v>-6.01</v>
       </c>
+      <c r="J101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -3605,6 +3710,7 @@
       <c r="I102" t="n">
         <v>-4.91</v>
       </c>
+      <c r="J102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -3636,6 +3742,7 @@
       <c r="I103" t="n">
         <v>-6.46</v>
       </c>
+      <c r="J103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -3667,6 +3774,7 @@
       <c r="I104" t="n">
         <v>-5.69</v>
       </c>
+      <c r="J104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -3698,6 +3806,7 @@
       <c r="I105" t="n">
         <v>-7.13</v>
       </c>
+      <c r="J105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -3729,6 +3838,7 @@
       <c r="I106" t="n">
         <v>-5.27</v>
       </c>
+      <c r="J106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -3760,6 +3870,7 @@
       <c r="I107" t="n">
         <v>-1.23</v>
       </c>
+      <c r="J107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -3791,6 +3902,7 @@
       <c r="I108" t="n">
         <v>-7.47</v>
       </c>
+      <c r="J108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -3822,6 +3934,7 @@
       <c r="I109" t="n">
         <v>-5.94</v>
       </c>
+      <c r="J109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -3853,6 +3966,7 @@
       <c r="I110" t="n">
         <v>-3.3</v>
       </c>
+      <c r="J110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -3884,6 +3998,7 @@
       <c r="I111" t="n">
         <v>-8.029999999999999</v>
       </c>
+      <c r="J111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -3915,6 +4030,7 @@
       <c r="I112" t="n">
         <v>-1.16</v>
       </c>
+      <c r="J112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -3946,6 +4062,7 @@
       <c r="I113" t="n">
         <v>-6.44</v>
       </c>
+      <c r="J113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -3977,6 +4094,7 @@
       <c r="I114" t="n">
         <v>-4.86</v>
       </c>
+      <c r="J114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -4008,6 +4126,7 @@
       <c r="I115" t="n">
         <v>-6.6</v>
       </c>
+      <c r="J115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -4039,6 +4158,7 @@
       <c r="I116" t="n">
         <v>-6.95</v>
       </c>
+      <c r="J116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -4070,6 +4190,7 @@
       <c r="I117" t="n">
         <v>-5.44</v>
       </c>
+      <c r="J117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -4101,6 +4222,7 @@
       <c r="I118" t="n">
         <v>-7.64</v>
       </c>
+      <c r="J118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -4132,6 +4254,7 @@
       <c r="I119" t="n">
         <v>-4.42</v>
       </c>
+      <c r="J119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -4163,6 +4286,7 @@
       <c r="I120" t="n">
         <v>-8.56</v>
       </c>
+      <c r="J120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -4194,6 +4318,7 @@
       <c r="I121" t="n">
         <v>-6.89</v>
       </c>
+      <c r="J121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -4225,6 +4350,7 @@
       <c r="I122" t="n">
         <v>-7.93</v>
       </c>
+      <c r="J122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -4256,6 +4382,7 @@
       <c r="I123" t="n">
         <v>-8.41</v>
       </c>
+      <c r="J123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -4287,6 +4414,7 @@
       <c r="I124" t="n">
         <v>5.49</v>
       </c>
+      <c r="J124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
@@ -4318,6 +4446,7 @@
       <c r="I125" t="n">
         <v>-7.89</v>
       </c>
+      <c r="J125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -4349,6 +4478,7 @@
       <c r="I126" t="n">
         <v>-7.89</v>
       </c>
+      <c r="J126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -4380,6 +4510,7 @@
       <c r="I127" t="n">
         <v>-6.71</v>
       </c>
+      <c r="J127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
@@ -4411,6 +4542,7 @@
       <c r="I128" t="n">
         <v>-3.4</v>
       </c>
+      <c r="J128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
@@ -4442,6 +4574,7 @@
       <c r="I129" t="n">
         <v>-7.62</v>
       </c>
+      <c r="J129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
@@ -4473,6 +4606,7 @@
       <c r="I130" t="n">
         <v>-2.48</v>
       </c>
+      <c r="J130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
@@ -4504,6 +4638,7 @@
       <c r="I131" t="n">
         <v>-2.14</v>
       </c>
+      <c r="J131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
@@ -4535,6 +4670,7 @@
       <c r="I132" t="n">
         <v>-7.52</v>
       </c>
+      <c r="J132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
@@ -4566,6 +4702,7 @@
       <c r="I133" t="n">
         <v>-6.82</v>
       </c>
+      <c r="J133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
@@ -4597,6 +4734,7 @@
       <c r="I134" t="n">
         <v>-7.09</v>
       </c>
+      <c r="J134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
@@ -4628,6 +4766,7 @@
       <c r="I135" t="n">
         <v>-4.54</v>
       </c>
+      <c r="J135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
@@ -4659,6 +4798,7 @@
       <c r="I136" t="n">
         <v>-7.45</v>
       </c>
+      <c r="J136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
@@ -4690,6 +4830,7 @@
       <c r="I137" t="n">
         <v>-4.97</v>
       </c>
+      <c r="J137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
@@ -4721,6 +4862,7 @@
       <c r="I138" t="n">
         <v>-7.4</v>
       </c>
+      <c r="J138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
@@ -4752,6 +4894,7 @@
       <c r="I139" t="n">
         <v>-8.119999999999999</v>
       </c>
+      <c r="J139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
@@ -4783,6 +4926,7 @@
       <c r="I140" t="n">
         <v>-1.36</v>
       </c>
+      <c r="J140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
@@ -4814,6 +4958,7 @@
       <c r="I141" t="n">
         <v>-6.69</v>
       </c>
+      <c r="J141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
@@ -4845,6 +4990,7 @@
       <c r="I142" t="n">
         <v>-4.21</v>
       </c>
+      <c r="J142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
@@ -4876,6 +5022,7 @@
       <c r="I143" t="n">
         <v>-6.98</v>
       </c>
+      <c r="J143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
@@ -4907,6 +5054,7 @@
       <c r="I144" t="n">
         <v>-5.16</v>
       </c>
+      <c r="J144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
@@ -4938,6 +5086,7 @@
       <c r="I145" t="n">
         <v>-6.72</v>
       </c>
+      <c r="J145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
@@ -4969,6 +5118,7 @@
       <c r="I146" t="n">
         <v>-7.22</v>
       </c>
+      <c r="J146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
@@ -5000,6 +5150,7 @@
       <c r="I147" t="n">
         <v>-6.88</v>
       </c>
+      <c r="J147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
@@ -5031,6 +5182,7 @@
       <c r="I148" t="n">
         <v>-2.91</v>
       </c>
+      <c r="J148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
@@ -5062,6 +5214,7 @@
       <c r="I149" t="n">
         <v>-4.75</v>
       </c>
+      <c r="J149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
@@ -5093,6 +5246,7 @@
       <c r="I150" t="n">
         <v>-7.57</v>
       </c>
+      <c r="J150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
@@ -5124,6 +5278,7 @@
       <c r="I151" t="n">
         <v>2.63</v>
       </c>
+      <c r="J151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
@@ -5155,6 +5310,7 @@
       <c r="I152" t="n">
         <v>-7.47</v>
       </c>
+      <c r="J152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
@@ -5186,6 +5342,7 @@
       <c r="I153" t="n">
         <v>-7.42</v>
       </c>
+      <c r="J153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
@@ -5217,6 +5374,7 @@
       <c r="I154" t="n">
         <v>0.59</v>
       </c>
+      <c r="J154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
@@ -5248,6 +5406,7 @@
       <c r="I155" t="n">
         <v>-6.55</v>
       </c>
+      <c r="J155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
@@ -5279,6 +5438,7 @@
       <c r="I156" t="n">
         <v>-6.09</v>
       </c>
+      <c r="J156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
@@ -5310,6 +5470,7 @@
       <c r="I157" t="n">
         <v>-7.73</v>
       </c>
+      <c r="J157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
@@ -5341,6 +5502,7 @@
       <c r="I158" t="n">
         <v>-7.21</v>
       </c>
+      <c r="J158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
@@ -5372,6 +5534,7 @@
       <c r="I159" t="n">
         <v>-2.5</v>
       </c>
+      <c r="J159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
@@ -5403,6 +5566,7 @@
       <c r="I160" t="n">
         <v>-6.93</v>
       </c>
+      <c r="J160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
@@ -5434,6 +5598,7 @@
       <c r="I161" t="n">
         <v>-7.26</v>
       </c>
+      <c r="J161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
@@ -5465,6 +5630,7 @@
       <c r="I162" t="n">
         <v>-6.81</v>
       </c>
+      <c r="J162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
@@ -5496,6 +5662,7 @@
       <c r="I163" t="n">
         <v>-7.45</v>
       </c>
+      <c r="J163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
@@ -5527,6 +5694,7 @@
       <c r="I164" t="n">
         <v>-8.720000000000001</v>
       </c>
+      <c r="J164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
@@ -5558,6 +5726,7 @@
       <c r="I165" t="n">
         <v>1.6</v>
       </c>
+      <c r="J165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
@@ -5589,6 +5758,7 @@
       <c r="I166" t="n">
         <v>-3.79</v>
       </c>
+      <c r="J166" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>